<commit_message>
updates on results from reound 4
</commit_message>
<xml_diff>
--- a/part_3_cohere/analysis/Round_4_scibert/dense_answer_relevance_results_data.xlsx
+++ b/part_3_cohere/analysis/Round_4_scibert/dense_answer_relevance_results_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/poppyriddle/Documents/Github/Research_proposal/part_3_cohere/analysis/Round_4_scibert/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF32DDA4-89AB-A045-BC4A-BDD4D6176482}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CA0D2D6-F565-6F45-9268-9D3657913CF4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="30300" yWindow="500" windowWidth="30240" windowHeight="18880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="raw_data" sheetId="1" r:id="rId1"/>
@@ -967,8 +967,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D71"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -988,183 +988,231 @@
         <v>86</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="208" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" ht="320" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>2</v>
+        <v>22</v>
       </c>
       <c r="C2" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="272" x14ac:dyDescent="0.2">
+      <c r="A3" s="1">
+        <v>24</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="335" x14ac:dyDescent="0.2">
+      <c r="A4" s="1">
+        <v>38</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="320" x14ac:dyDescent="0.2">
+      <c r="A5" s="1">
+        <v>52</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="320" x14ac:dyDescent="0.2">
+      <c r="A6" s="1">
+        <v>66</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="224" x14ac:dyDescent="0.2">
+      <c r="A7" s="1">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" ht="224" x14ac:dyDescent="0.2">
-      <c r="A3" s="1">
-        <v>1</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ht="208" x14ac:dyDescent="0.2">
-      <c r="A4" s="1">
-        <v>2</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" ht="224" x14ac:dyDescent="0.2">
-      <c r="A5" s="1">
-        <v>3</v>
-      </c>
-      <c r="B5" s="3" t="s">
+      <c r="B7" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C7" s="3" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" ht="288" x14ac:dyDescent="0.2">
-      <c r="A6" s="1">
-        <v>4</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" ht="208" x14ac:dyDescent="0.2">
-      <c r="A7" s="1">
-        <v>5</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" ht="304" x14ac:dyDescent="0.2">
+      <c r="D7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="208" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
-        <v>6</v>
+        <v>17</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" ht="304" x14ac:dyDescent="0.2">
+        <v>33</v>
+      </c>
+      <c r="D8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="256" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
-        <v>7</v>
+        <v>31</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" ht="272" x14ac:dyDescent="0.2">
+        <v>47</v>
+      </c>
+      <c r="D9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="240" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
+        <v>45</v>
+      </c>
+      <c r="B10" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B10" s="3" t="s">
-        <v>18</v>
-      </c>
       <c r="C10" s="3" t="s">
-        <v>19</v>
+        <v>61</v>
+      </c>
+      <c r="D10">
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="256" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
-        <v>9</v>
+        <v>59</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" ht="320" x14ac:dyDescent="0.2">
+        <v>75</v>
+      </c>
+      <c r="D11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="304" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" ht="320" x14ac:dyDescent="0.2">
+        <v>29</v>
+      </c>
+      <c r="D12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="240" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
-        <v>11</v>
+        <v>27</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" ht="272" x14ac:dyDescent="0.2">
+        <v>43</v>
+      </c>
+      <c r="D13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="176" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
-        <v>12</v>
+        <v>41</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>27</v>
+        <v>57</v>
+      </c>
+      <c r="D14">
+        <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="304" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
-        <v>13</v>
+        <v>55</v>
       </c>
       <c r="B15" s="3" t="s">
         <v>28</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" ht="224" x14ac:dyDescent="0.2">
+        <v>71</v>
+      </c>
+      <c r="D15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="350" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
-        <v>14</v>
+        <v>69</v>
       </c>
       <c r="B16" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="D16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="208" x14ac:dyDescent="0.2">
+      <c r="A17" s="1">
         <v>2</v>
       </c>
-      <c r="C16" s="3" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" ht="335" x14ac:dyDescent="0.2">
-      <c r="A17" s="1">
-        <v>15</v>
-      </c>
       <c r="B17" s="3" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" ht="240" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+      <c r="D17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="240" x14ac:dyDescent="0.2">
       <c r="A18" s="1">
         <v>16</v>
       </c>
@@ -1174,591 +1222,756 @@
       <c r="C18" s="3" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" ht="208" x14ac:dyDescent="0.2">
+      <c r="D18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="256" x14ac:dyDescent="0.2">
       <c r="A19" s="1">
-        <v>17</v>
+        <v>30</v>
       </c>
       <c r="B19" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="D19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="256" x14ac:dyDescent="0.2">
+      <c r="A20" s="1">
+        <v>44</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="D20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="272" x14ac:dyDescent="0.2">
+      <c r="A21" s="1">
+        <v>58</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="D21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="272" x14ac:dyDescent="0.2">
+      <c r="A22" s="1">
         <v>8</v>
       </c>
-      <c r="C19" s="3" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" ht="288" x14ac:dyDescent="0.2">
-      <c r="A20" s="1">
+      <c r="B22" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="B20" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C20" s="3" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" ht="208" x14ac:dyDescent="0.2">
-      <c r="A21" s="1">
+      <c r="C22" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B21" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C21" s="3" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" ht="224" x14ac:dyDescent="0.2">
-      <c r="A22" s="1">
-        <v>20</v>
-      </c>
-      <c r="B22" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="C22" s="3" t="s">
+      <c r="D22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="304" x14ac:dyDescent="0.2">
+      <c r="A23" s="1">
+        <v>22</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="D23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="288" x14ac:dyDescent="0.2">
+      <c r="A24" s="1">
         <v>36</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" ht="335" x14ac:dyDescent="0.2">
-      <c r="A23" s="1">
-        <v>21</v>
-      </c>
-      <c r="B23" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="C23" s="3" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" ht="304" x14ac:dyDescent="0.2">
-      <c r="A24" s="1">
-        <v>22</v>
       </c>
       <c r="B24" s="3" t="s">
         <v>18</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" ht="288" x14ac:dyDescent="0.2">
+        <v>52</v>
+      </c>
+      <c r="D24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="288" x14ac:dyDescent="0.2">
       <c r="A25" s="1">
-        <v>23</v>
+        <v>50</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" ht="272" x14ac:dyDescent="0.2">
+        <v>66</v>
+      </c>
+      <c r="D25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" ht="272" x14ac:dyDescent="0.2">
       <c r="A26" s="1">
-        <v>24</v>
+        <v>64</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" ht="365" x14ac:dyDescent="0.2">
+        <v>80</v>
+      </c>
+      <c r="D26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" ht="320" x14ac:dyDescent="0.2">
       <c r="A27" s="1">
-        <v>25</v>
+        <v>11</v>
       </c>
       <c r="B27" s="3" t="s">
         <v>24</v>
       </c>
       <c r="C27" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" ht="365" x14ac:dyDescent="0.2">
+      <c r="A28" s="1">
+        <v>25</v>
+      </c>
+      <c r="B28" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C28" s="3" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="28" spans="1:3" ht="240" x14ac:dyDescent="0.2">
-      <c r="A28" s="1">
-        <v>26</v>
-      </c>
-      <c r="B28" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="C28" s="3" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" ht="240" x14ac:dyDescent="0.2">
+      <c r="D28">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" ht="365" x14ac:dyDescent="0.2">
       <c r="A29" s="1">
-        <v>27</v>
+        <v>39</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" ht="208" x14ac:dyDescent="0.2">
+        <v>55</v>
+      </c>
+      <c r="D29">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" ht="365" x14ac:dyDescent="0.2">
       <c r="A30" s="1">
-        <v>28</v>
+        <v>53</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>2</v>
+        <v>24</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" ht="240" x14ac:dyDescent="0.2">
+        <v>69</v>
+      </c>
+      <c r="D30">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" ht="335" x14ac:dyDescent="0.2">
       <c r="A31" s="1">
-        <v>29</v>
+        <v>67</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>4</v>
+        <v>24</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" ht="256" x14ac:dyDescent="0.2">
+        <v>83</v>
+      </c>
+      <c r="D31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" ht="256" x14ac:dyDescent="0.2">
       <c r="A32" s="1">
-        <v>30</v>
+        <v>9</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>6</v>
+        <v>20</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" ht="256" x14ac:dyDescent="0.2">
+        <v>21</v>
+      </c>
+      <c r="D32">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" ht="288" x14ac:dyDescent="0.2">
       <c r="A33" s="1">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" ht="256" x14ac:dyDescent="0.2">
+        <v>39</v>
+      </c>
+      <c r="D33">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" ht="256" x14ac:dyDescent="0.2">
       <c r="A34" s="1">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" ht="208" x14ac:dyDescent="0.2">
+        <v>53</v>
+      </c>
+      <c r="D34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" ht="240" x14ac:dyDescent="0.2">
       <c r="A35" s="1">
-        <v>33</v>
+        <v>51</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" ht="224" x14ac:dyDescent="0.2">
+        <v>67</v>
+      </c>
+      <c r="D35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" ht="272" x14ac:dyDescent="0.2">
       <c r="A36" s="1">
-        <v>34</v>
+        <v>65</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" ht="304" x14ac:dyDescent="0.2">
+        <v>81</v>
+      </c>
+      <c r="D36">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" ht="304" x14ac:dyDescent="0.2">
       <c r="A37" s="1">
-        <v>35</v>
+        <v>7</v>
       </c>
       <c r="B37" s="3" t="s">
         <v>16</v>
       </c>
       <c r="C37" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D37">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" ht="335" x14ac:dyDescent="0.2">
+      <c r="A38" s="1">
+        <v>21</v>
+      </c>
+      <c r="B38" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C38" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="D38">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" ht="304" x14ac:dyDescent="0.2">
+      <c r="A39" s="1">
+        <v>35</v>
+      </c>
+      <c r="B39" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C39" s="3" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="38" spans="1:3" ht="288" x14ac:dyDescent="0.2">
-      <c r="A38" s="1">
-        <v>36</v>
-      </c>
-      <c r="B38" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="C38" s="3" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" ht="256" x14ac:dyDescent="0.2">
-      <c r="A39" s="1">
-        <v>37</v>
-      </c>
-      <c r="B39" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="C39" s="3" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" ht="335" x14ac:dyDescent="0.2">
+      <c r="D39">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" ht="304" x14ac:dyDescent="0.2">
       <c r="A40" s="1">
-        <v>38</v>
+        <v>49</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" ht="365" x14ac:dyDescent="0.2">
+        <v>65</v>
+      </c>
+      <c r="D40">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" ht="288" x14ac:dyDescent="0.2">
       <c r="A41" s="1">
-        <v>39</v>
+        <v>63</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" ht="256" x14ac:dyDescent="0.2">
+        <v>79</v>
+      </c>
+      <c r="D41">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" ht="272" x14ac:dyDescent="0.2">
       <c r="A42" s="1">
-        <v>40</v>
+        <v>12</v>
       </c>
       <c r="B42" s="3" t="s">
         <v>26</v>
       </c>
       <c r="C42" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D42">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" ht="240" x14ac:dyDescent="0.2">
+      <c r="A43" s="1">
+        <v>26</v>
+      </c>
+      <c r="B43" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C43" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="D43">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" ht="256" x14ac:dyDescent="0.2">
+      <c r="A44" s="1">
+        <v>40</v>
+      </c>
+      <c r="B44" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C44" s="3" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="43" spans="1:3" ht="176" x14ac:dyDescent="0.2">
-      <c r="A43" s="1">
-        <v>41</v>
-      </c>
-      <c r="B43" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="C43" s="3" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" ht="192" x14ac:dyDescent="0.2">
-      <c r="A44" s="1">
-        <v>42</v>
-      </c>
-      <c r="B44" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C44" s="3" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3" ht="256" x14ac:dyDescent="0.2">
+      <c r="D44">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" ht="256" x14ac:dyDescent="0.2">
       <c r="A45" s="1">
-        <v>43</v>
+        <v>54</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>4</v>
+        <v>26</v>
       </c>
       <c r="C45" s="3" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3" ht="256" x14ac:dyDescent="0.2">
+        <v>70</v>
+      </c>
+      <c r="D45">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" ht="272" x14ac:dyDescent="0.2">
       <c r="A46" s="1">
-        <v>44</v>
+        <v>68</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>6</v>
+        <v>26</v>
       </c>
       <c r="C46" s="3" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3" ht="240" x14ac:dyDescent="0.2">
+        <v>84</v>
+      </c>
+      <c r="D46">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" ht="208" x14ac:dyDescent="0.2">
       <c r="A47" s="1">
-        <v>45</v>
+        <v>5</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="C47" s="3" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3" ht="240" x14ac:dyDescent="0.2">
+        <v>13</v>
+      </c>
+      <c r="D47">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" ht="208" x14ac:dyDescent="0.2">
       <c r="A48" s="1">
-        <v>46</v>
+        <v>19</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C48" s="3" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3" ht="208" x14ac:dyDescent="0.2">
+        <v>35</v>
+      </c>
+      <c r="D48">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" ht="208" x14ac:dyDescent="0.2">
       <c r="A49" s="1">
-        <v>47</v>
+        <v>33</v>
       </c>
       <c r="B49" s="3" t="s">
         <v>12</v>
       </c>
       <c r="C49" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="D49">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" ht="208" x14ac:dyDescent="0.2">
+      <c r="A50" s="1">
+        <v>47</v>
+      </c>
+      <c r="B50" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C50" s="3" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="50" spans="1:3" ht="224" x14ac:dyDescent="0.2">
-      <c r="A50" s="1">
+      <c r="D50">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" ht="240" x14ac:dyDescent="0.2">
+      <c r="A51" s="1">
+        <v>61</v>
+      </c>
+      <c r="B51" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C51" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="D51">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" ht="304" x14ac:dyDescent="0.2">
+      <c r="A52" s="1">
+        <v>6</v>
+      </c>
+      <c r="B52" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C52" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D52">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" ht="224" x14ac:dyDescent="0.2">
+      <c r="A53" s="1">
+        <v>20</v>
+      </c>
+      <c r="B53" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C53" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="D53">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" ht="224" x14ac:dyDescent="0.2">
+      <c r="A54" s="1">
+        <v>34</v>
+      </c>
+      <c r="B54" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C54" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="D54">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" ht="224" x14ac:dyDescent="0.2">
+      <c r="A55" s="1">
         <v>48</v>
       </c>
-      <c r="B50" s="3" t="s">
+      <c r="B55" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C50" s="3" t="s">
+      <c r="C55" s="3" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="51" spans="1:3" ht="304" x14ac:dyDescent="0.2">
-      <c r="A51" s="1">
-        <v>49</v>
-      </c>
-      <c r="B51" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="C51" s="3" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="52" spans="1:3" ht="288" x14ac:dyDescent="0.2">
-      <c r="A52" s="1">
-        <v>50</v>
-      </c>
-      <c r="B52" s="3" t="s">
+      <c r="D55">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" ht="288" x14ac:dyDescent="0.2">
+      <c r="A56" s="1">
+        <v>62</v>
+      </c>
+      <c r="B56" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C56" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="D56">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" ht="288" x14ac:dyDescent="0.2">
+      <c r="A57" s="1">
+        <v>4</v>
+      </c>
+      <c r="B57" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C57" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D57">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" ht="288" x14ac:dyDescent="0.2">
+      <c r="A58" s="1">
         <v>18</v>
       </c>
-      <c r="C52" s="3" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="53" spans="1:3" ht="240" x14ac:dyDescent="0.2">
-      <c r="A53" s="1">
-        <v>51</v>
-      </c>
-      <c r="B53" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="C53" s="3" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="54" spans="1:3" ht="320" x14ac:dyDescent="0.2">
-      <c r="A54" s="1">
-        <v>52</v>
-      </c>
-      <c r="B54" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="C54" s="3" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="55" spans="1:3" ht="365" x14ac:dyDescent="0.2">
-      <c r="A55" s="1">
-        <v>53</v>
-      </c>
-      <c r="B55" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="C55" s="3" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="56" spans="1:3" ht="256" x14ac:dyDescent="0.2">
-      <c r="A56" s="1">
-        <v>54</v>
-      </c>
-      <c r="B56" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="C56" s="3" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="57" spans="1:3" ht="304" x14ac:dyDescent="0.2">
-      <c r="A57" s="1">
-        <v>55</v>
-      </c>
-      <c r="B57" s="3" t="s">
+      <c r="B58" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C58" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="D58">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" ht="256" x14ac:dyDescent="0.2">
+      <c r="A59" s="1">
+        <v>32</v>
+      </c>
+      <c r="B59" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C59" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="D59">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" ht="240" x14ac:dyDescent="0.2">
+      <c r="A60" s="1">
+        <v>46</v>
+      </c>
+      <c r="B60" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C60" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="D60">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" ht="256" x14ac:dyDescent="0.2">
+      <c r="A61" s="1">
+        <v>60</v>
+      </c>
+      <c r="B61" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C61" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="D61">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" ht="224" x14ac:dyDescent="0.2">
+      <c r="A62" s="1">
+        <v>1</v>
+      </c>
+      <c r="B62" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C62" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D62">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" ht="335" x14ac:dyDescent="0.2">
+      <c r="A63" s="1">
+        <v>15</v>
+      </c>
+      <c r="B63" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C63" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="D63">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" ht="240" x14ac:dyDescent="0.2">
+      <c r="A64" s="1">
+        <v>29</v>
+      </c>
+      <c r="B64" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C64" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="D64">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" ht="256" x14ac:dyDescent="0.2">
+      <c r="A65" s="1">
+        <v>43</v>
+      </c>
+      <c r="B65" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C65" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="D65">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" ht="224" x14ac:dyDescent="0.2">
+      <c r="A66" s="1">
+        <v>57</v>
+      </c>
+      <c r="B66" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C66" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="D66">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" ht="208" x14ac:dyDescent="0.2">
+      <c r="A67" s="1">
+        <v>0</v>
+      </c>
+      <c r="B67" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C67" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D67">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" ht="224" x14ac:dyDescent="0.2">
+      <c r="A68" s="1">
+        <v>14</v>
+      </c>
+      <c r="B68" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C68" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D68">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" ht="208" x14ac:dyDescent="0.2">
+      <c r="A69" s="1">
         <v>28</v>
       </c>
-      <c r="C57" s="3" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="58" spans="1:3" ht="208" x14ac:dyDescent="0.2">
-      <c r="A58" s="1">
+      <c r="B69" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C69" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="D69">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" ht="192" x14ac:dyDescent="0.2">
+      <c r="A70" s="1">
+        <v>42</v>
+      </c>
+      <c r="B70" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C70" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="D70">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" ht="208" x14ac:dyDescent="0.2">
+      <c r="A71" s="1">
         <v>56</v>
       </c>
-      <c r="B58" s="3" t="s">
+      <c r="B71" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C58" s="3" t="s">
+      <c r="C71" s="3" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="59" spans="1:3" ht="224" x14ac:dyDescent="0.2">
-      <c r="A59" s="1">
-        <v>57</v>
-      </c>
-      <c r="B59" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C59" s="3" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="60" spans="1:3" ht="272" x14ac:dyDescent="0.2">
-      <c r="A60" s="1">
-        <v>58</v>
-      </c>
-      <c r="B60" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C60" s="3" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="61" spans="1:3" ht="256" x14ac:dyDescent="0.2">
-      <c r="A61" s="1">
-        <v>59</v>
-      </c>
-      <c r="B61" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C61" s="3" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="62" spans="1:3" ht="256" x14ac:dyDescent="0.2">
-      <c r="A62" s="1">
-        <v>60</v>
-      </c>
-      <c r="B62" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C62" s="3" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="63" spans="1:3" ht="240" x14ac:dyDescent="0.2">
-      <c r="A63" s="1">
-        <v>61</v>
-      </c>
-      <c r="B63" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C63" s="3" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="64" spans="1:3" ht="288" x14ac:dyDescent="0.2">
-      <c r="A64" s="1">
-        <v>62</v>
-      </c>
-      <c r="B64" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="C64" s="3" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="65" spans="1:3" ht="288" x14ac:dyDescent="0.2">
-      <c r="A65" s="1">
-        <v>63</v>
-      </c>
-      <c r="B65" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="C65" s="3" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="66" spans="1:3" ht="272" x14ac:dyDescent="0.2">
-      <c r="A66" s="1">
-        <v>64</v>
-      </c>
-      <c r="B66" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="C66" s="3" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="67" spans="1:3" ht="272" x14ac:dyDescent="0.2">
-      <c r="A67" s="1">
-        <v>65</v>
-      </c>
-      <c r="B67" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="C67" s="3" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="68" spans="1:3" ht="320" x14ac:dyDescent="0.2">
-      <c r="A68" s="1">
-        <v>66</v>
-      </c>
-      <c r="B68" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="C68" s="3" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="69" spans="1:3" ht="335" x14ac:dyDescent="0.2">
-      <c r="A69" s="1">
-        <v>67</v>
-      </c>
-      <c r="B69" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="C69" s="3" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="70" spans="1:3" ht="272" x14ac:dyDescent="0.2">
-      <c r="A70" s="1">
-        <v>68</v>
-      </c>
-      <c r="B70" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="C70" s="3" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="71" spans="1:3" ht="350" x14ac:dyDescent="0.2">
-      <c r="A71" s="1">
-        <v>69</v>
-      </c>
-      <c r="B71" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="C71" s="3" t="s">
-        <v>85</v>
+      <c r="D71">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D71">
+    <sortCondition ref="B2:B71"/>
+  </sortState>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
updated Round 4 results
</commit_message>
<xml_diff>
--- a/part_3_cohere/analysis/Round_4_scibert/dense_answer_relevance_results_data.xlsx
+++ b/part_3_cohere/analysis/Round_4_scibert/dense_answer_relevance_results_data.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/poppyriddle/Documents/Github/Research_proposal/part_3_cohere/analysis/Round_4_scibert/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CA0D2D6-F565-6F45-9268-9D3657913CF4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29A73E5A-6754-6044-AB3C-4A9355836BF7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="30300" yWindow="500" windowWidth="30240" windowHeight="18880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="raw_data" sheetId="1" r:id="rId1"/>
+    <sheet name="raw data" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>

</xml_diff>